<commit_message>
Actualizar funcionalidades de salud financiera
</commit_message>
<xml_diff>
--- a/excel/usuarios_funcionalidades.xlsx
+++ b/excel/usuarios_funcionalidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>clave</t>
   </si>
@@ -51,9 +51,6 @@
     <t>CASA LEO FERRETERIA</t>
   </si>
   <si>
-    <t>cliente_premium</t>
-  </si>
-  <si>
     <t>CASA GABY</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>RAFAEL FERRETERIA</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -449,7 +449,7 @@
         <v>20166</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -457,13 +457,13 @@
         <v>20114</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>20114</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -471,10 +471,24 @@
         <v>1817</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20246</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
+      </c>
+      <c r="C7">
+        <v>20246</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar configuración usuarios y funcionalidades
</commit_message>
<xml_diff>
--- a/excel/usuarios_funcionalidades.xlsx
+++ b/excel/usuarios_funcionalidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>clave</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>RAFAEL FERRETERIA</t>
+  </si>
+  <si>
+    <t>CHRISTIAN</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +421,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12345</v>
+        <v>1218</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -429,7 +432,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1234</v>
+        <v>1959</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -440,27 +443,24 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20166</v>
+        <v>5625</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>20166</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20114</v>
+        <v>20166</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>20114</v>
+        <v>20166</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -468,27 +468,41 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1817</v>
+        <v>20114</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>20114</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>1817</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>20246</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>20246</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
+      <c r="D8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>